<commit_message>
Filled D and E columns
</commit_message>
<xml_diff>
--- a/7 Dalam Negeri/Elaun Hotel atau Lojing Dalam Negeri.xlsx
+++ b/7 Dalam Negeri/Elaun Hotel atau Lojing Dalam Negeri.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="305">
   <si>
     <t>Gred</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>DG4</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
   <si>
     <t>DG5</t>
@@ -1562,7 +1565,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1579,6 +1582,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2116,8 +2122,8 @@
   <sheetPr/>
   <dimension ref="A1:E298"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -2128,17 +2134,17 @@
     <col min="5" max="5" width="26.7777777777778" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2506,6 +2512,12 @@
       <c r="B40" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C40">
+        <v>290</v>
+      </c>
+      <c r="D40">
+        <v>110</v>
+      </c>
       <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:5">
@@ -2515,6 +2527,12 @@
       <c r="B41" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C41">
+        <v>370</v>
+      </c>
+      <c r="D41">
+        <v>130</v>
+      </c>
       <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:5">
@@ -2524,7 +2542,12 @@
       <c r="B42" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="5"/>
+      <c r="C42">
+        <v>420</v>
+      </c>
+      <c r="D42" s="5">
+        <v>140</v>
+      </c>
       <c r="E42" s="2"/>
     </row>
     <row r="43" spans="1:5">
@@ -2534,83 +2557,137 @@
       <c r="B43" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C43" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" t="s">
+        <v>48</v>
+      </c>
       <c r="E43" s="2"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C44">
+        <v>320</v>
+      </c>
+      <c r="D44">
+        <v>120</v>
       </c>
       <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C45">
+        <v>320</v>
+      </c>
+      <c r="D45">
+        <v>120</v>
       </c>
       <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C46">
+        <v>370</v>
+      </c>
+      <c r="D46">
+        <v>130</v>
       </c>
       <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C47">
+        <v>290</v>
+      </c>
+      <c r="D47">
+        <v>110</v>
       </c>
       <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" t="s">
+        <v>48</v>
       </c>
       <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C49" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" t="s">
+        <v>48</v>
       </c>
       <c r="E49" s="2"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C50" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50" t="s">
+        <v>48</v>
       </c>
       <c r="E50" s="2"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C51">
+        <v>290</v>
+      </c>
+      <c r="D51">
+        <v>110</v>
       </c>
       <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>5</v>
@@ -2619,7 +2696,7 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>5</v>
@@ -2629,7 +2706,7 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>5</v>
@@ -2639,7 +2716,7 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>5</v>
@@ -2648,7 +2725,7 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>5</v>
@@ -2657,7 +2734,7 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>5</v>
@@ -2666,7 +2743,7 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>5</v>
@@ -2675,7 +2752,7 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>12</v>
@@ -2684,7 +2761,7 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>12</v>
@@ -2693,7 +2770,7 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>12</v>
@@ -2702,7 +2779,7 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>5</v>
@@ -2711,7 +2788,7 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>5</v>
@@ -2721,7 +2798,7 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>5</v>
@@ -2731,7 +2808,7 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>5</v>
@@ -2741,7 +2818,7 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>5</v>
@@ -2750,7 +2827,7 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>5</v>
@@ -2759,7 +2836,7 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>5</v>
@@ -2768,7 +2845,7 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>5</v>
@@ -2777,7 +2854,7 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>12</v>
@@ -2786,7 +2863,7 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>12</v>
@@ -2795,7 +2872,7 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>12</v>
@@ -2804,7 +2881,7 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>5</v>
@@ -2813,7 +2890,7 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>12</v>
@@ -2822,7 +2899,7 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>5</v>
@@ -2831,7 +2908,7 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>5</v>
@@ -2840,7 +2917,7 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>5</v>
@@ -2849,7 +2926,7 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>5</v>
@@ -2858,7 +2935,7 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>5</v>
@@ -2868,7 +2945,7 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>5</v>
@@ -2878,7 +2955,7 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>5</v>
@@ -2888,7 +2965,7 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>5</v>
@@ -2898,7 +2975,7 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>5</v>
@@ -2907,7 +2984,7 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>5</v>
@@ -2916,7 +2993,7 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>5</v>
@@ -2925,7 +3002,7 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>5</v>
@@ -2934,7 +3011,7 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>5</v>
@@ -2943,7 +3020,7 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>5</v>
@@ -2952,7 +3029,7 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>5</v>
@@ -2962,7 +3039,7 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>5</v>
@@ -2972,7 +3049,7 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>12</v>
@@ -2981,7 +3058,7 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>12</v>
@@ -2990,7 +3067,7 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>12</v>
@@ -2999,7 +3076,7 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>12</v>
@@ -3008,7 +3085,7 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>12</v>
@@ -3017,7 +3094,7 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>12</v>
@@ -3026,7 +3103,7 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>5</v>
@@ -3035,7 +3112,7 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>5</v>
@@ -3044,7 +3121,7 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>5</v>
@@ -3053,7 +3130,7 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>5</v>
@@ -3062,7 +3139,7 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>12</v>
@@ -3072,7 +3149,7 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>5</v>
@@ -3081,7 +3158,7 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>5</v>
@@ -3090,7 +3167,7 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>5</v>
@@ -3100,7 +3177,7 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>5</v>
@@ -3109,7 +3186,7 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>5</v>
@@ -3118,7 +3195,7 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>5</v>
@@ -3128,7 +3205,7 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>5</v>
@@ -3138,7 +3215,7 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>12</v>
@@ -3147,7 +3224,7 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>12</v>
@@ -3156,7 +3233,7 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>12</v>
@@ -3165,7 +3242,7 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>5</v>
@@ -3174,7 +3251,7 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>5</v>
@@ -3183,7 +3260,7 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>5</v>
@@ -3193,7 +3270,7 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>5</v>
@@ -3203,7 +3280,7 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>5</v>
@@ -3213,7 +3290,7 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>5</v>
@@ -3222,7 +3299,7 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>5</v>
@@ -3231,7 +3308,7 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>5</v>
@@ -3240,7 +3317,7 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>5</v>
@@ -3249,7 +3326,7 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>5</v>
@@ -3258,7 +3335,7 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>5</v>
@@ -3267,7 +3344,7 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>5</v>
@@ -3276,7 +3353,7 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>12</v>
@@ -3285,7 +3362,7 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>12</v>
@@ -3294,7 +3371,7 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>12</v>
@@ -3303,7 +3380,7 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>12</v>
@@ -3312,7 +3389,7 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>12</v>
@@ -3321,7 +3398,7 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>12</v>
@@ -3330,7 +3407,7 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>12</v>
@@ -3339,7 +3416,7 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>12</v>
@@ -3348,7 +3425,7 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>12</v>
@@ -3357,7 +3434,7 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>12</v>
@@ -3367,7 +3444,7 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>12</v>
@@ -3377,7 +3454,7 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>5</v>
@@ -3386,7 +3463,7 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>5</v>
@@ -3395,7 +3472,7 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>5</v>
@@ -3404,7 +3481,7 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>5</v>
@@ -3413,7 +3490,7 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>5</v>
@@ -3422,7 +3499,7 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>5</v>
@@ -3432,7 +3509,7 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>5</v>
@@ -3442,7 +3519,7 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>5</v>
@@ -3452,7 +3529,7 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>12</v>
@@ -3461,7 +3538,7 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>5</v>
@@ -3470,7 +3547,7 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>12</v>
@@ -3479,7 +3556,7 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>12</v>
@@ -3488,7 +3565,7 @@
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>12</v>
@@ -3497,7 +3574,7 @@
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>5</v>
@@ -3506,7 +3583,7 @@
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>12</v>
@@ -3515,7 +3592,7 @@
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>12</v>
@@ -3524,7 +3601,7 @@
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>5</v>
@@ -3533,7 +3610,7 @@
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>5</v>
@@ -3542,7 +3619,7 @@
     </row>
     <row r="153" spans="1:5">
       <c r="A153" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>5</v>
@@ -3551,7 +3628,7 @@
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>5</v>
@@ -3560,7 +3637,7 @@
     </row>
     <row r="155" spans="1:5">
       <c r="A155" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>5</v>
@@ -3570,7 +3647,7 @@
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>5</v>
@@ -3579,7 +3656,7 @@
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>5</v>
@@ -3588,7 +3665,7 @@
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>5</v>
@@ -3598,7 +3675,7 @@
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>5</v>
@@ -3608,7 +3685,7 @@
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>5</v>
@@ -3618,7 +3695,7 @@
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>5</v>
@@ -3627,7 +3704,7 @@
     </row>
     <row r="162" spans="1:5">
       <c r="A162" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>5</v>
@@ -3636,7 +3713,7 @@
     </row>
     <row r="163" spans="1:5">
       <c r="A163" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>5</v>
@@ -3645,7 +3722,7 @@
     </row>
     <row r="164" spans="1:5">
       <c r="A164" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>5</v>
@@ -3654,7 +3731,7 @@
     </row>
     <row r="165" spans="1:5">
       <c r="A165" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>5</v>
@@ -3663,7 +3740,7 @@
     </row>
     <row r="166" spans="1:5">
       <c r="A166" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>5</v>
@@ -3672,7 +3749,7 @@
     </row>
     <row r="167" spans="1:5">
       <c r="A167" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>12</v>
@@ -3681,7 +3758,7 @@
     </row>
     <row r="168" spans="1:5">
       <c r="A168" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>12</v>
@@ -3690,7 +3767,7 @@
     </row>
     <row r="169" spans="1:5">
       <c r="A169" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>12</v>
@@ -3700,7 +3777,7 @@
     </row>
     <row r="170" spans="1:5">
       <c r="A170" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>12</v>
@@ -3710,7 +3787,7 @@
     </row>
     <row r="171" spans="1:5">
       <c r="A171" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>5</v>
@@ -3720,7 +3797,7 @@
     </row>
     <row r="172" spans="1:5">
       <c r="A172" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>5</v>
@@ -3729,7 +3806,7 @@
     </row>
     <row r="173" spans="1:5">
       <c r="A173" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>5</v>
@@ -3738,7 +3815,7 @@
     </row>
     <row r="174" spans="1:5">
       <c r="A174" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>5</v>
@@ -3747,7 +3824,7 @@
     </row>
     <row r="175" spans="1:5">
       <c r="A175" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>5</v>
@@ -3756,7 +3833,7 @@
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>5</v>
@@ -3765,7 +3842,7 @@
     </row>
     <row r="177" spans="1:5">
       <c r="A177" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>5</v>
@@ -3774,7 +3851,7 @@
     </row>
     <row r="178" spans="1:5">
       <c r="A178" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>5</v>
@@ -3784,7 +3861,7 @@
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>5</v>
@@ -3794,7 +3871,7 @@
     </row>
     <row r="180" spans="1:5">
       <c r="A180" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>5</v>
@@ -3804,7 +3881,7 @@
     </row>
     <row r="181" spans="1:5">
       <c r="A181" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>5</v>
@@ -3813,7 +3890,7 @@
     </row>
     <row r="182" spans="1:5">
       <c r="A182" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>5</v>
@@ -3822,7 +3899,7 @@
     </row>
     <row r="183" spans="1:5">
       <c r="A183" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>5</v>
@@ -3831,7 +3908,7 @@
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>5</v>
@@ -3840,7 +3917,7 @@
     </row>
     <row r="185" spans="1:5">
       <c r="A185" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>5</v>
@@ -3849,7 +3926,7 @@
     </row>
     <row r="186" spans="1:5">
       <c r="A186" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>5</v>
@@ -3858,7 +3935,7 @@
     </row>
     <row r="187" spans="1:5">
       <c r="A187" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>5</v>
@@ -3867,7 +3944,7 @@
     </row>
     <row r="188" spans="1:5">
       <c r="A188" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>5</v>
@@ -3876,7 +3953,7 @@
     </row>
     <row r="189" spans="1:5">
       <c r="A189" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>5</v>
@@ -3885,7 +3962,7 @@
     </row>
     <row r="190" spans="1:5">
       <c r="A190" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>5</v>
@@ -3895,7 +3972,7 @@
     </row>
     <row r="191" spans="1:5">
       <c r="A191" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>5</v>
@@ -3905,7 +3982,7 @@
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>5</v>
@@ -3914,7 +3991,7 @@
     </row>
     <row r="193" spans="1:5">
       <c r="A193" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>12</v>
@@ -3923,7 +4000,7 @@
     </row>
     <row r="194" spans="1:5">
       <c r="A194" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>12</v>
@@ -3932,7 +4009,7 @@
     </row>
     <row r="195" spans="1:5">
       <c r="A195" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>12</v>
@@ -3941,7 +4018,7 @@
     </row>
     <row r="196" spans="1:5">
       <c r="A196" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>12</v>
@@ -3950,7 +4027,7 @@
     </row>
     <row r="197" spans="1:5">
       <c r="A197" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>12</v>
@@ -3959,7 +4036,7 @@
     </row>
     <row r="198" spans="1:5">
       <c r="A198" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>12</v>
@@ -3968,7 +4045,7 @@
     </row>
     <row r="199" spans="1:5">
       <c r="A199" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>12</v>
@@ -3977,7 +4054,7 @@
     </row>
     <row r="200" spans="1:5">
       <c r="A200" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>12</v>
@@ -3986,7 +4063,7 @@
     </row>
     <row r="201" spans="1:5">
       <c r="A201" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>12</v>
@@ -3995,7 +4072,7 @@
     </row>
     <row r="202" spans="1:5">
       <c r="A202" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>12</v>
@@ -4005,7 +4082,7 @@
     </row>
     <row r="203" spans="1:5">
       <c r="A203" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>12</v>
@@ -4015,7 +4092,7 @@
     </row>
     <row r="204" spans="1:5">
       <c r="A204" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>12</v>
@@ -4025,7 +4102,7 @@
     </row>
     <row r="205" spans="1:5">
       <c r="A205" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>5</v>
@@ -4034,7 +4111,7 @@
     </row>
     <row r="206" spans="1:5">
       <c r="A206" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>12</v>
@@ -4043,7 +4120,7 @@
     </row>
     <row r="207" spans="1:5">
       <c r="A207" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>5</v>
@@ -4052,7 +4129,7 @@
     </row>
     <row r="208" spans="1:5">
       <c r="A208" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>12</v>
@@ -4061,7 +4138,7 @@
     </row>
     <row r="209" spans="1:5">
       <c r="A209" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>12</v>
@@ -4070,7 +4147,7 @@
     </row>
     <row r="210" spans="1:5">
       <c r="A210" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>12</v>
@@ -4079,7 +4156,7 @@
     </row>
     <row r="211" spans="1:5">
       <c r="A211" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>5</v>
@@ -4088,7 +4165,7 @@
     </row>
     <row r="212" spans="1:5">
       <c r="A212" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>12</v>
@@ -4097,7 +4174,7 @@
     </row>
     <row r="213" spans="1:5">
       <c r="A213" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>5</v>
@@ -4106,7 +4183,7 @@
     </row>
     <row r="214" spans="1:5">
       <c r="A214" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>5</v>
@@ -4115,7 +4192,7 @@
     </row>
     <row r="215" spans="1:5">
       <c r="A215" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>5</v>
@@ -4124,7 +4201,7 @@
     </row>
     <row r="216" spans="1:5">
       <c r="A216" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>5</v>
@@ -4133,7 +4210,7 @@
     </row>
     <row r="217" spans="1:5">
       <c r="A217" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>5</v>
@@ -4143,7 +4220,7 @@
     </row>
     <row r="218" spans="1:5">
       <c r="A218" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>5</v>
@@ -4153,7 +4230,7 @@
     </row>
     <row r="219" spans="1:5">
       <c r="A219" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>5</v>
@@ -4163,7 +4240,7 @@
     </row>
     <row r="220" spans="1:5">
       <c r="A220" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>5</v>
@@ -4172,7 +4249,7 @@
     </row>
     <row r="221" spans="1:5">
       <c r="A221" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>5</v>
@@ -4181,7 +4258,7 @@
     </row>
     <row r="222" spans="1:5">
       <c r="A222" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>5</v>
@@ -4190,7 +4267,7 @@
     </row>
     <row r="223" spans="1:5">
       <c r="A223" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>5</v>
@@ -4199,7 +4276,7 @@
     </row>
     <row r="224" spans="1:5">
       <c r="A224" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>5</v>
@@ -4208,7 +4285,7 @@
     </row>
     <row r="225" spans="1:5">
       <c r="A225" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>12</v>
@@ -4217,7 +4294,7 @@
     </row>
     <row r="226" spans="1:5">
       <c r="A226" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>12</v>
@@ -4226,7 +4303,7 @@
     </row>
     <row r="227" spans="1:5">
       <c r="A227" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>5</v>
@@ -4235,7 +4312,7 @@
     </row>
     <row r="228" spans="1:5">
       <c r="A228" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>5</v>
@@ -4244,7 +4321,7 @@
     </row>
     <row r="229" spans="1:5">
       <c r="A229" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>5</v>
@@ -4253,7 +4330,7 @@
     </row>
     <row r="230" spans="1:5">
       <c r="A230" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>5</v>
@@ -4262,7 +4339,7 @@
     </row>
     <row r="231" spans="1:5">
       <c r="A231" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>5</v>
@@ -4271,7 +4348,7 @@
     </row>
     <row r="232" spans="1:5">
       <c r="A232" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>5</v>
@@ -4280,7 +4357,7 @@
     </row>
     <row r="233" spans="1:5">
       <c r="A233" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>5</v>
@@ -4289,7 +4366,7 @@
     </row>
     <row r="234" spans="1:5">
       <c r="A234" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B234" s="1" t="s">
         <v>5</v>
@@ -4298,7 +4375,7 @@
     </row>
     <row r="235" spans="1:5">
       <c r="A235" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B235" s="1" t="s">
         <v>5</v>
@@ -4308,7 +4385,7 @@
     </row>
     <row r="236" spans="1:5">
       <c r="A236" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B236" s="1" t="s">
         <v>5</v>
@@ -4318,7 +4395,7 @@
     </row>
     <row r="237" spans="1:5">
       <c r="A237" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>5</v>
@@ -4327,7 +4404,7 @@
     </row>
     <row r="238" spans="1:5">
       <c r="A238" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>5</v>
@@ -4336,7 +4413,7 @@
     </row>
     <row r="239" spans="1:5">
       <c r="A239" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B239" s="1" t="s">
         <v>5</v>
@@ -4345,7 +4422,7 @@
     </row>
     <row r="240" spans="1:5">
       <c r="A240" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B240" s="1" t="s">
         <v>5</v>
@@ -4354,7 +4431,7 @@
     </row>
     <row r="241" spans="1:5">
       <c r="A241" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B241" s="1" t="s">
         <v>5</v>
@@ -4363,7 +4440,7 @@
     </row>
     <row r="242" spans="1:5">
       <c r="A242" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B242" s="1" t="s">
         <v>5</v>
@@ -4372,7 +4449,7 @@
     </row>
     <row r="243" spans="1:5">
       <c r="A243" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>5</v>
@@ -4381,7 +4458,7 @@
     </row>
     <row r="244" spans="1:5">
       <c r="A244" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B244" s="1" t="s">
         <v>12</v>
@@ -4390,7 +4467,7 @@
     </row>
     <row r="245" spans="1:5">
       <c r="A245" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B245" s="1" t="s">
         <v>12</v>
@@ -4399,7 +4476,7 @@
     </row>
     <row r="246" spans="1:5">
       <c r="A246" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B246" s="1" t="s">
         <v>12</v>
@@ -4408,7 +4485,7 @@
     </row>
     <row r="247" spans="1:5">
       <c r="A247" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>12</v>
@@ -4417,7 +4494,7 @@
     </row>
     <row r="248" spans="1:5">
       <c r="A248" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>12</v>
@@ -4426,7 +4503,7 @@
     </row>
     <row r="249" spans="1:5">
       <c r="A249" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B249" s="1" t="s">
         <v>12</v>
@@ -4435,7 +4512,7 @@
     </row>
     <row r="250" spans="1:5">
       <c r="A250" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B250" s="1" t="s">
         <v>12</v>
@@ -4445,7 +4522,7 @@
     </row>
     <row r="251" spans="1:5">
       <c r="A251" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B251" s="1" t="s">
         <v>12</v>
@@ -4455,7 +4532,7 @@
     </row>
     <row r="252" spans="1:5">
       <c r="A252" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B252" s="1" t="s">
         <v>5</v>
@@ -4464,7 +4541,7 @@
     </row>
     <row r="253" spans="1:5">
       <c r="A253" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B253" s="1" t="s">
         <v>5</v>
@@ -4473,7 +4550,7 @@
     </row>
     <row r="254" spans="1:5">
       <c r="A254" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B254" s="1" t="s">
         <v>5</v>
@@ -4482,7 +4559,7 @@
     </row>
     <row r="255" spans="1:5">
       <c r="A255" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B255" s="1" t="s">
         <v>5</v>
@@ -4491,7 +4568,7 @@
     </row>
     <row r="256" spans="1:5">
       <c r="A256" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B256" s="1" t="s">
         <v>5</v>
@@ -4500,7 +4577,7 @@
     </row>
     <row r="257" spans="1:5">
       <c r="A257" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B257" s="1" t="s">
         <v>5</v>
@@ -4509,7 +4586,7 @@
     </row>
     <row r="258" spans="1:5">
       <c r="A258" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B258" s="1" t="s">
         <v>12</v>
@@ -4518,7 +4595,7 @@
     </row>
     <row r="259" spans="1:5">
       <c r="A259" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B259" s="1" t="s">
         <v>12</v>
@@ -4527,10 +4604,10 @@
     </row>
     <row r="260" spans="1:5">
       <c r="A260" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C260" s="4"/>
       <c r="D260" s="4"/>
@@ -4538,10 +4615,10 @@
     </row>
     <row r="261" spans="1:5">
       <c r="A261" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B261" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="B261" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="C261" s="5"/>
       <c r="D261" s="5"/>
@@ -4549,10 +4626,10 @@
     </row>
     <row r="262" spans="1:5">
       <c r="A262" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C262" s="4"/>
       <c r="D262" s="4"/>
@@ -4560,10 +4637,10 @@
     </row>
     <row r="263" spans="1:5">
       <c r="A263" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C263" s="5"/>
       <c r="D263" s="5"/>
@@ -4571,10 +4648,10 @@
     </row>
     <row r="264" spans="1:5">
       <c r="A264" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C264" s="5"/>
       <c r="D264" s="5"/>
@@ -4582,10 +4659,10 @@
     </row>
     <row r="265" spans="1:5">
       <c r="A265" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C265" s="5"/>
       <c r="D265" s="5"/>
@@ -4593,10 +4670,10 @@
     </row>
     <row r="266" spans="1:5">
       <c r="A266" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C266" s="5"/>
       <c r="D266" s="5"/>
@@ -4604,10 +4681,10 @@
     </row>
     <row r="267" spans="1:5">
       <c r="A267" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C267" s="5"/>
       <c r="D267" s="5"/>
@@ -4615,10 +4692,10 @@
     </row>
     <row r="268" spans="1:5">
       <c r="A268" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C268" s="5"/>
       <c r="D268" s="5"/>
@@ -4626,7 +4703,7 @@
     </row>
     <row r="269" spans="1:5">
       <c r="A269" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B269" s="1" t="s">
         <v>5</v>
@@ -4635,7 +4712,7 @@
     </row>
     <row r="270" spans="1:5">
       <c r="A270" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>5</v>
@@ -4644,7 +4721,7 @@
     </row>
     <row r="271" spans="1:5">
       <c r="A271" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>5</v>
@@ -4654,7 +4731,7 @@
     </row>
     <row r="272" spans="1:5">
       <c r="A272" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>5</v>
@@ -4664,7 +4741,7 @@
     </row>
     <row r="273" spans="1:5">
       <c r="A273" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>5</v>
@@ -4674,7 +4751,7 @@
     </row>
     <row r="274" spans="1:5">
       <c r="A274" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B274" s="1" t="s">
         <v>5</v>
@@ -4683,7 +4760,7 @@
     </row>
     <row r="275" spans="1:5">
       <c r="A275" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B275" s="1" t="s">
         <v>5</v>
@@ -4692,7 +4769,7 @@
     </row>
     <row r="276" spans="1:5">
       <c r="A276" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B276" s="1" t="s">
         <v>5</v>
@@ -4701,7 +4778,7 @@
     </row>
     <row r="277" spans="1:5">
       <c r="A277" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B277" s="1" t="s">
         <v>5</v>
@@ -4710,7 +4787,7 @@
     </row>
     <row r="278" spans="1:5">
       <c r="A278" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B278" s="1" t="s">
         <v>5</v>
@@ -4719,7 +4796,7 @@
     </row>
     <row r="279" spans="1:5">
       <c r="A279" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B279" s="1" t="s">
         <v>5</v>
@@ -4728,7 +4805,7 @@
     </row>
     <row r="280" spans="1:5">
       <c r="A280" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B280" s="1" t="s">
         <v>5</v>
@@ -4737,7 +4814,7 @@
     </row>
     <row r="281" spans="1:5">
       <c r="A281" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B281" s="1" t="s">
         <v>5</v>
@@ -4746,7 +4823,7 @@
     </row>
     <row r="282" spans="1:5">
       <c r="A282" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B282" s="1" t="s">
         <v>5</v>
@@ -4756,7 +4833,7 @@
     </row>
     <row r="283" spans="1:5">
       <c r="A283" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B283" s="1" t="s">
         <v>12</v>
@@ -4765,7 +4842,7 @@
     </row>
     <row r="284" spans="1:5">
       <c r="A284" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B284" s="1" t="s">
         <v>12</v>
@@ -4774,7 +4851,7 @@
     </row>
     <row r="285" spans="1:5">
       <c r="A285" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B285" s="1" t="s">
         <v>12</v>
@@ -4783,7 +4860,7 @@
     </row>
     <row r="286" spans="1:5">
       <c r="A286" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B286" s="1" t="s">
         <v>12</v>
@@ -4792,7 +4869,7 @@
     </row>
     <row r="287" spans="1:5">
       <c r="A287" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B287" s="1" t="s">
         <v>12</v>
@@ -4801,7 +4878,7 @@
     </row>
     <row r="288" spans="1:5">
       <c r="A288" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B288" s="1" t="s">
         <v>12</v>
@@ -4810,7 +4887,7 @@
     </row>
     <row r="289" spans="1:5">
       <c r="A289" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B289" s="1" t="s">
         <v>12</v>
@@ -4819,7 +4896,7 @@
     </row>
     <row r="290" spans="1:5">
       <c r="A290" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B290" s="1" t="s">
         <v>12</v>
@@ -4829,7 +4906,7 @@
     </row>
     <row r="291" spans="1:5">
       <c r="A291" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B291" s="1" t="s">
         <v>12</v>
@@ -4839,7 +4916,7 @@
     </row>
     <row r="292" spans="1:5">
       <c r="A292" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B292" s="1" t="s">
         <v>5</v>
@@ -4848,7 +4925,7 @@
     </row>
     <row r="293" spans="1:5">
       <c r="A293" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B293" s="1" t="s">
         <v>12</v>
@@ -4857,7 +4934,7 @@
     </row>
     <row r="294" spans="1:5">
       <c r="A294" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B294" s="1" t="s">
         <v>5</v>
@@ -4866,7 +4943,7 @@
     </row>
     <row r="295" spans="1:5">
       <c r="A295" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B295" s="1" t="s">
         <v>5</v>
@@ -4875,7 +4952,7 @@
     </row>
     <row r="296" spans="1:5">
       <c r="A296" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B296" s="1" t="s">
         <v>5</v>
@@ -4884,7 +4961,7 @@
     </row>
     <row r="297" spans="1:5">
       <c r="A297" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B297" s="1" t="s">
         <v>5</v>
@@ -4893,7 +4970,7 @@
     </row>
     <row r="298" spans="1:5">
       <c r="A298" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B298" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update Elaun Hotel atau Lojing Dalam Negeri.xlsx
</commit_message>
<xml_diff>
--- a/7 Dalam Negeri/Elaun Hotel atau Lojing Dalam Negeri.xlsx
+++ b/7 Dalam Negeri/Elaun Hotel atau Lojing Dalam Negeri.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="11520" windowHeight="9000"/>
+    <workbookView windowWidth="11520" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="306">
   <si>
     <t>Gred</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>E14</t>
+  </si>
+  <si>
+    <t>Sebenar (Deluxe/Superior)</t>
   </si>
   <si>
     <t>E2</t>
@@ -1565,7 +1568,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1582,9 +1585,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2122,8 +2122,8 @@
   <sheetPr/>
   <dimension ref="A1:E298"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="C172" sqref="C172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -2512,10 +2512,10 @@
       <c r="B40" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="2">
         <v>290</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="2">
         <v>110</v>
       </c>
       <c r="E40" s="2"/>
@@ -2527,10 +2527,10 @@
       <c r="B41" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="2">
         <v>370</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="2">
         <v>130</v>
       </c>
       <c r="E41" s="2"/>
@@ -2542,10 +2542,10 @@
       <c r="B42" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="2">
         <v>420</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D42" s="2">
         <v>140</v>
       </c>
       <c r="E42" s="2"/>
@@ -2557,10 +2557,10 @@
       <c r="B43" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E43" s="2"/>
@@ -2572,10 +2572,10 @@
       <c r="B44" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="2">
         <v>320</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="2">
         <v>120</v>
       </c>
       <c r="E44" s="2"/>
@@ -2587,10 +2587,10 @@
       <c r="B45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="2">
         <v>320</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="2">
         <v>120</v>
       </c>
       <c r="E45" s="2"/>
@@ -2602,10 +2602,10 @@
       <c r="B46" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="2">
         <v>370</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="2">
         <v>130</v>
       </c>
       <c r="E46" s="2"/>
@@ -2617,10 +2617,10 @@
       <c r="B47" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="2">
         <v>290</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="2">
         <v>110</v>
       </c>
       <c r="E47" s="2"/>
@@ -2632,10 +2632,10 @@
       <c r="B48" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E48" s="2"/>
@@ -2647,10 +2647,10 @@
       <c r="B49" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E49" s="2"/>
@@ -2662,10 +2662,10 @@
       <c r="B50" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E50" s="2"/>
@@ -2677,10 +2677,10 @@
       <c r="B51" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="2">
         <v>290</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="2">
         <v>110</v>
       </c>
       <c r="E51" s="2"/>
@@ -2692,6 +2692,12 @@
       <c r="B52" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C52" s="2">
+        <v>370</v>
+      </c>
+      <c r="D52" s="2">
+        <v>130</v>
+      </c>
       <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:5">
@@ -2701,7 +2707,12 @@
       <c r="B53" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D53" s="5"/>
+      <c r="C53" s="2">
+        <v>420</v>
+      </c>
+      <c r="D53" s="2">
+        <v>140</v>
+      </c>
       <c r="E53" s="2"/>
     </row>
     <row r="54" spans="1:5">
@@ -2711,1177 +2722,1907 @@
       <c r="B54" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D54" s="5"/>
+      <c r="C54" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" s="2">
+        <v>160</v>
+      </c>
       <c r="E54" s="2"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C55" s="2">
+        <v>290</v>
+      </c>
+      <c r="D55" s="2">
+        <v>110</v>
       </c>
       <c r="E55" s="2"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C56" s="2">
+        <v>320</v>
+      </c>
+      <c r="D56" s="2">
+        <v>120</v>
       </c>
       <c r="E56" s="2"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="E57" s="2"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C58" s="2">
+        <v>370</v>
+      </c>
+      <c r="D58" s="2">
+        <v>120</v>
       </c>
       <c r="E58" s="2"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C59" t="s">
+        <v>48</v>
+      </c>
+      <c r="D59" t="s">
+        <v>48</v>
       </c>
       <c r="E59" s="2"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C60" s="2">
+        <v>320</v>
+      </c>
+      <c r="D60" s="2">
+        <v>120</v>
       </c>
       <c r="E60" s="2"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C61" s="2">
+        <v>370</v>
+      </c>
+      <c r="D61" s="2">
+        <v>130</v>
       </c>
       <c r="E61" s="2"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C62" s="2">
+        <v>370</v>
+      </c>
+      <c r="D62" s="2">
+        <v>130</v>
       </c>
       <c r="E62" s="2"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D63" s="5"/>
+      <c r="C63" s="2">
+        <v>420</v>
+      </c>
+      <c r="D63" s="2">
+        <v>140</v>
+      </c>
       <c r="E63" s="2"/>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D64" s="5"/>
+      <c r="C64" s="2">
+        <v>460</v>
+      </c>
+      <c r="D64" s="2">
+        <v>150</v>
+      </c>
       <c r="E64" s="2"/>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D65" s="5"/>
+      <c r="C65" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D65" s="5">
+        <v>160</v>
+      </c>
       <c r="E65" s="2"/>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C66">
+        <v>320</v>
+      </c>
+      <c r="D66">
+        <v>120</v>
       </c>
       <c r="E66" s="2"/>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C67">
+        <v>320</v>
+      </c>
+      <c r="D67">
+        <v>120</v>
       </c>
       <c r="E67" s="2"/>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C68">
+        <v>320</v>
+      </c>
+      <c r="D68">
+        <v>120</v>
       </c>
       <c r="E68" s="2"/>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C69">
+        <v>370</v>
+      </c>
+      <c r="D69">
+        <v>130</v>
       </c>
       <c r="E69" s="2"/>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C70">
+        <v>320</v>
+      </c>
+      <c r="D70">
+        <v>120</v>
       </c>
       <c r="E70" s="2"/>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C71">
+        <v>370</v>
+      </c>
+      <c r="D71">
+        <v>130</v>
       </c>
       <c r="E71" s="2"/>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C72">
+        <v>370</v>
+      </c>
+      <c r="D72">
+        <v>130</v>
       </c>
       <c r="E72" s="2"/>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C73">
+        <v>290</v>
+      </c>
+      <c r="D73">
+        <v>110</v>
       </c>
       <c r="E73" s="2"/>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C74">
+        <v>290</v>
+      </c>
+      <c r="D74">
+        <v>110</v>
       </c>
       <c r="E74" s="2"/>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C75">
+        <v>290</v>
+      </c>
+      <c r="D75">
+        <v>110</v>
       </c>
       <c r="E75" s="2"/>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C76">
+        <v>290</v>
+      </c>
+      <c r="D76">
+        <v>110</v>
       </c>
       <c r="E76" s="2"/>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C77">
+        <v>290</v>
+      </c>
+      <c r="D77">
+        <v>110</v>
       </c>
       <c r="E77" s="2"/>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C78">
+        <v>370</v>
+      </c>
+      <c r="D78">
+        <v>130</v>
       </c>
       <c r="E78" s="2"/>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D79" s="5"/>
+      <c r="C79">
+        <v>420</v>
+      </c>
+      <c r="D79" s="5">
+        <v>140</v>
+      </c>
       <c r="E79" s="2"/>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D80" s="5"/>
+      <c r="C80">
+        <v>420</v>
+      </c>
+      <c r="D80" s="5">
+        <v>140</v>
+      </c>
       <c r="E80" s="2"/>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D81" s="5"/>
+      <c r="C81">
+        <v>460</v>
+      </c>
+      <c r="D81" s="5">
+        <v>150</v>
+      </c>
       <c r="E81" s="2"/>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D82" s="5"/>
+      <c r="C82" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D82" s="5">
+        <v>160</v>
+      </c>
       <c r="E82" s="2"/>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C83">
+        <v>290</v>
+      </c>
+      <c r="D83">
+        <v>110</v>
       </c>
       <c r="E83" s="2"/>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C84">
+        <v>290</v>
+      </c>
+      <c r="D84">
+        <v>110</v>
       </c>
       <c r="E84" s="2"/>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C85">
+        <v>320</v>
+      </c>
+      <c r="D85">
+        <v>120</v>
       </c>
       <c r="E85" s="2"/>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C86">
+        <v>320</v>
+      </c>
+      <c r="D86">
+        <v>120</v>
       </c>
       <c r="E86" s="2"/>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C87">
+        <v>320</v>
+      </c>
+      <c r="D87">
+        <v>120</v>
       </c>
       <c r="E87" s="2"/>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C88">
+        <v>370</v>
+      </c>
+      <c r="D88">
+        <v>130</v>
       </c>
       <c r="E88" s="2"/>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D89" s="5"/>
+      <c r="C89">
+        <v>420</v>
+      </c>
+      <c r="D89" s="5">
+        <v>140</v>
+      </c>
       <c r="E89" s="2"/>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D90" s="5"/>
+      <c r="C90" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D90" s="5">
+        <v>160</v>
+      </c>
       <c r="E90" s="2"/>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C91">
+        <v>290</v>
+      </c>
+      <c r="D91">
+        <v>110</v>
       </c>
       <c r="E91" s="2"/>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C92">
+        <v>290</v>
+      </c>
+      <c r="D92">
+        <v>110</v>
       </c>
       <c r="E92" s="2"/>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C93">
+        <v>290</v>
+      </c>
+      <c r="D93">
+        <v>110</v>
       </c>
       <c r="E93" s="2"/>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C94">
+        <v>320</v>
+      </c>
+      <c r="D94">
+        <v>120</v>
       </c>
       <c r="E94" s="2"/>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C95">
+        <v>370</v>
+      </c>
+      <c r="D95">
+        <v>130</v>
       </c>
       <c r="E95" s="2"/>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C96">
+        <v>370</v>
+      </c>
+      <c r="D96">
+        <v>130</v>
       </c>
       <c r="E96" s="2"/>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C97">
+        <v>370</v>
+      </c>
+      <c r="D97">
+        <v>130</v>
       </c>
       <c r="E97" s="2"/>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C98">
+        <v>420</v>
+      </c>
+      <c r="D98" s="5">
+        <v>140</v>
       </c>
       <c r="E98" s="2"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C99">
+        <v>460</v>
+      </c>
+      <c r="D99" s="5">
+        <v>150</v>
       </c>
       <c r="E99" s="2"/>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D100" s="5">
+        <v>160</v>
       </c>
       <c r="E100" s="2"/>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D101" s="5"/>
+      <c r="C101">
+        <v>460</v>
+      </c>
+      <c r="D101" s="5">
+        <v>150</v>
+      </c>
       <c r="E101" s="2"/>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C102">
+        <v>370</v>
+      </c>
+      <c r="D102">
+        <v>130</v>
       </c>
       <c r="E102" s="2"/>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C103">
+        <v>290</v>
+      </c>
+      <c r="D103">
+        <v>110</v>
       </c>
       <c r="E103" s="2"/>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D104" s="5"/>
+      <c r="C104">
+        <v>420</v>
+      </c>
+      <c r="D104" s="5">
+        <v>140</v>
+      </c>
       <c r="E104" s="2"/>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105">
+        <v>290</v>
+      </c>
+      <c r="D105">
         <v>110</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="E105" s="2"/>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C106">
+        <v>290</v>
+      </c>
+      <c r="D106">
+        <v>110</v>
       </c>
       <c r="E106" s="2"/>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D107" s="5"/>
+      <c r="C107">
+        <v>420</v>
+      </c>
+      <c r="D107" s="5">
+        <v>140</v>
+      </c>
       <c r="E107" s="2"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D108" s="5"/>
+      <c r="C108" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D108" s="5">
+        <v>160</v>
+      </c>
       <c r="E108" s="2"/>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C109">
+        <v>290</v>
+      </c>
+      <c r="D109">
+        <v>110</v>
       </c>
       <c r="E109" s="2"/>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C110">
+        <v>290</v>
+      </c>
+      <c r="D110">
+        <v>110</v>
       </c>
       <c r="E110" s="2"/>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C111">
+        <v>290</v>
+      </c>
+      <c r="D111">
+        <v>110</v>
       </c>
       <c r="E111" s="2"/>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C112">
+        <v>290</v>
+      </c>
+      <c r="D112">
+        <v>110</v>
       </c>
       <c r="E112" s="2"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C113">
+        <v>370</v>
+      </c>
+      <c r="D113">
+        <v>130</v>
       </c>
       <c r="E113" s="2"/>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D114" s="5"/>
+      <c r="C114">
+        <v>420</v>
+      </c>
+      <c r="D114" s="5">
+        <v>140</v>
+      </c>
       <c r="E114" s="2"/>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D115" s="5"/>
+      <c r="C115">
+        <v>460</v>
+      </c>
+      <c r="D115" s="5">
+        <v>150</v>
+      </c>
       <c r="E115" s="2"/>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D116" s="5"/>
+      <c r="C116" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D116" s="5">
+        <v>160</v>
+      </c>
       <c r="E116" s="2"/>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C117">
+        <v>290</v>
+      </c>
+      <c r="D117">
+        <v>110</v>
       </c>
       <c r="E117" s="2"/>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C118">
+        <v>290</v>
+      </c>
+      <c r="D118">
+        <v>110</v>
       </c>
       <c r="E118" s="2"/>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C119">
+        <v>320</v>
+      </c>
+      <c r="D119">
+        <v>120</v>
       </c>
       <c r="E119" s="2"/>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C120">
+        <v>320</v>
+      </c>
+      <c r="D120">
+        <v>120</v>
       </c>
       <c r="E120" s="2"/>
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C121">
+        <v>320</v>
+      </c>
+      <c r="D121">
+        <v>120</v>
       </c>
       <c r="E121" s="2"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C122">
+        <v>370</v>
+      </c>
+      <c r="D122">
+        <v>130</v>
       </c>
       <c r="E122" s="2"/>
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C123">
+        <v>290</v>
+      </c>
+      <c r="D123">
+        <v>110</v>
       </c>
       <c r="E123" s="2"/>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C124">
+        <v>260</v>
+      </c>
+      <c r="D124">
+        <v>100</v>
       </c>
       <c r="E124" s="2"/>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C125">
+        <v>290</v>
+      </c>
+      <c r="D125">
+        <v>110</v>
       </c>
       <c r="E125" s="2"/>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C126">
+        <v>290</v>
+      </c>
+      <c r="D126">
+        <v>110</v>
       </c>
       <c r="E126" s="2"/>
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C127">
+        <v>290</v>
+      </c>
+      <c r="D127">
+        <v>110</v>
       </c>
       <c r="E127" s="2"/>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C128">
+        <v>320</v>
+      </c>
+      <c r="D128">
+        <v>120</v>
       </c>
       <c r="E128" s="2"/>
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C129">
+        <v>320</v>
+      </c>
+      <c r="D129">
+        <v>120</v>
       </c>
       <c r="E129" s="2"/>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C130">
+        <v>320</v>
+      </c>
+      <c r="D130">
+        <v>120</v>
       </c>
       <c r="E130" s="2"/>
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C131">
+        <v>370</v>
+      </c>
+      <c r="D131">
+        <v>130</v>
       </c>
       <c r="E131" s="2"/>
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C132">
+        <v>370</v>
+      </c>
+      <c r="D132">
+        <v>130</v>
       </c>
       <c r="E132" s="2"/>
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D133" s="5"/>
+      <c r="C133">
+        <v>420</v>
+      </c>
+      <c r="D133" s="5">
+        <v>140</v>
+      </c>
       <c r="E133" s="2"/>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D134" s="5"/>
+      <c r="C134">
+        <v>460</v>
+      </c>
+      <c r="D134" s="5">
+        <v>150</v>
+      </c>
       <c r="E134" s="2"/>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C135">
+        <v>290</v>
+      </c>
+      <c r="D135">
+        <v>110</v>
       </c>
       <c r="E135" s="2"/>
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C136">
+        <v>290</v>
+      </c>
+      <c r="D136">
+        <v>110</v>
       </c>
       <c r="E136" s="2"/>
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C137">
+        <v>320</v>
+      </c>
+      <c r="D137">
+        <v>120</v>
       </c>
       <c r="E137" s="2"/>
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C138">
+        <v>290</v>
+      </c>
+      <c r="D138">
+        <v>110</v>
       </c>
       <c r="E138" s="2"/>
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C139">
+        <v>370</v>
+      </c>
+      <c r="D139">
+        <v>130</v>
       </c>
       <c r="E139" s="2"/>
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D140" s="5"/>
+      <c r="C140">
+        <v>370</v>
+      </c>
+      <c r="D140">
+        <v>130</v>
+      </c>
       <c r="E140" s="2"/>
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D141" s="5"/>
+      <c r="C141">
+        <v>370</v>
+      </c>
+      <c r="D141">
+        <v>130</v>
+      </c>
       <c r="E141" s="2"/>
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D142" s="5"/>
+      <c r="C142" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D142" s="5">
+        <v>160</v>
+      </c>
       <c r="E142" s="2"/>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C143">
+        <v>290</v>
+      </c>
+      <c r="D143">
+        <v>110</v>
       </c>
       <c r="E143" s="2"/>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C144">
+        <v>290</v>
+      </c>
+      <c r="D144">
+        <v>110</v>
       </c>
       <c r="E144" s="2"/>
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C145">
+        <v>290</v>
+      </c>
+      <c r="D145">
+        <v>110</v>
       </c>
       <c r="E145" s="2"/>
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C146">
+        <v>320</v>
+      </c>
+      <c r="D146">
+        <v>120</v>
       </c>
       <c r="E146" s="2"/>
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C147">
+        <v>320</v>
+      </c>
+      <c r="D147">
+        <v>120</v>
       </c>
       <c r="E147" s="2"/>
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C148">
+        <v>320</v>
+      </c>
+      <c r="D148">
+        <v>120</v>
       </c>
       <c r="E148" s="2"/>
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C149">
+        <v>320</v>
+      </c>
+      <c r="D149">
+        <v>120</v>
       </c>
       <c r="E149" s="2"/>
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C150">
+        <v>370</v>
+      </c>
+      <c r="D150">
+        <v>130</v>
       </c>
       <c r="E150" s="2"/>
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C151">
+        <v>320</v>
+      </c>
+      <c r="D151">
+        <v>120</v>
       </c>
       <c r="E151" s="2"/>
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C152">
+        <v>320</v>
+      </c>
+      <c r="D152">
+        <v>120</v>
       </c>
       <c r="E152" s="2"/>
     </row>
     <row r="153" spans="1:5">
       <c r="A153" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C153">
+        <v>320</v>
+      </c>
+      <c r="D153">
+        <v>120</v>
       </c>
       <c r="E153" s="2"/>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C154">
+        <v>370</v>
+      </c>
+      <c r="D154">
+        <v>130</v>
       </c>
       <c r="E154" s="2"/>
     </row>
     <row r="155" spans="1:5">
       <c r="A155" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D155" s="5">
         <v>160</v>
       </c>
-      <c r="B155" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D155" s="5"/>
       <c r="E155" s="2"/>
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C156">
+        <v>290</v>
+      </c>
+      <c r="D156">
+        <v>110</v>
       </c>
       <c r="E156" s="2"/>
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C157">
+        <v>370</v>
+      </c>
+      <c r="D157">
+        <v>130</v>
       </c>
       <c r="E157" s="2"/>
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D158" s="5"/>
+      <c r="C158">
+        <v>420</v>
+      </c>
+      <c r="D158" s="5">
+        <v>140</v>
+      </c>
       <c r="E158" s="2"/>
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D159" s="5"/>
+      <c r="C159">
+        <v>460</v>
+      </c>
+      <c r="D159" s="5">
+        <v>150</v>
+      </c>
       <c r="E159" s="2"/>
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D160" s="5"/>
+      <c r="C160" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D160" s="5">
+        <v>160</v>
+      </c>
       <c r="E160" s="2"/>
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C161">
+        <v>290</v>
+      </c>
+      <c r="D161">
+        <v>110</v>
       </c>
       <c r="E161" s="2"/>
     </row>
     <row r="162" spans="1:5">
       <c r="A162" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C162">
+        <v>290</v>
+      </c>
+      <c r="D162">
+        <v>110</v>
       </c>
       <c r="E162" s="2"/>
     </row>
     <row r="163" spans="1:5">
       <c r="A163" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C163">
+        <v>320</v>
+      </c>
+      <c r="D163">
+        <v>120</v>
       </c>
       <c r="E163" s="2"/>
     </row>
     <row r="164" spans="1:5">
       <c r="A164" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C164">
+        <v>320</v>
+      </c>
+      <c r="D164">
+        <v>120</v>
       </c>
       <c r="E164" s="2"/>
     </row>
     <row r="165" spans="1:5">
       <c r="A165" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C165">
+        <v>320</v>
+      </c>
+      <c r="D165">
+        <v>120</v>
       </c>
       <c r="E165" s="2"/>
     </row>
     <row r="166" spans="1:5">
       <c r="A166" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C166">
+        <v>370</v>
+      </c>
+      <c r="D166">
+        <v>130</v>
       </c>
       <c r="E166" s="2"/>
     </row>
     <row r="167" spans="1:5">
       <c r="A167" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C167">
+        <v>320</v>
+      </c>
+      <c r="D167">
+        <v>120</v>
       </c>
       <c r="E167" s="2"/>
     </row>
     <row r="168" spans="1:5">
       <c r="A168" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C168">
+        <v>370</v>
+      </c>
+      <c r="D168">
+        <v>130</v>
       </c>
       <c r="E168" s="2"/>
     </row>
     <row r="169" spans="1:5">
       <c r="A169" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D169" s="5"/>
+      <c r="C169">
+        <v>420</v>
+      </c>
+      <c r="D169" s="5">
+        <v>140</v>
+      </c>
       <c r="E169" s="2"/>
     </row>
     <row r="170" spans="1:5">
       <c r="A170" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D170" s="5"/>
+      <c r="C170">
+        <v>460</v>
+      </c>
+      <c r="D170" s="5">
+        <v>150</v>
+      </c>
       <c r="E170" s="2"/>
     </row>
     <row r="171" spans="1:5">
       <c r="A171" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D171" s="5"/>
+      <c r="C171">
+        <v>420</v>
+      </c>
+      <c r="D171" s="5">
+        <v>140</v>
+      </c>
       <c r="E171" s="2"/>
     </row>
     <row r="172" spans="1:5">
       <c r="A172" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C172">
+        <v>320</v>
+      </c>
+      <c r="D172">
+        <v>120</v>
       </c>
       <c r="E172" s="2"/>
     </row>
     <row r="173" spans="1:5">
       <c r="A173" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C173">
+        <v>320</v>
+      </c>
+      <c r="D173">
+        <v>120</v>
       </c>
       <c r="E173" s="2"/>
     </row>
     <row r="174" spans="1:5">
       <c r="A174" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C174">
+        <v>370</v>
+      </c>
+      <c r="D174">
+        <v>130</v>
       </c>
       <c r="E174" s="2"/>
     </row>
     <row r="175" spans="1:5">
       <c r="A175" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C175">
+        <v>290</v>
+      </c>
+      <c r="D175">
+        <v>110</v>
       </c>
       <c r="E175" s="2"/>
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C176">
+        <v>370</v>
+      </c>
+      <c r="D176">
+        <v>130</v>
       </c>
       <c r="E176" s="2"/>
     </row>
     <row r="177" spans="1:5">
       <c r="A177" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C177">
+        <v>420</v>
+      </c>
+      <c r="D177" s="5">
+        <v>140</v>
       </c>
       <c r="E177" s="2"/>
     </row>
     <row r="178" spans="1:5">
       <c r="A178" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D178" s="5"/>
+      <c r="C178">
+        <v>420</v>
+      </c>
+      <c r="D178" s="5">
+        <v>140</v>
+      </c>
       <c r="E178" s="2"/>
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D179" s="5"/>
+      <c r="C179">
+        <v>460</v>
+      </c>
+      <c r="D179" s="5">
+        <v>150</v>
+      </c>
       <c r="E179" s="2"/>
     </row>
     <row r="180" spans="1:5">
       <c r="A180" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D180" s="5"/>
+      <c r="C180" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D180" s="5">
+        <v>160</v>
+      </c>
       <c r="E180" s="2"/>
     </row>
     <row r="181" spans="1:5">
       <c r="A181" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>5</v>
@@ -3890,7 +4631,7 @@
     </row>
     <row r="182" spans="1:5">
       <c r="A182" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>5</v>
@@ -3899,7 +4640,7 @@
     </row>
     <row r="183" spans="1:5">
       <c r="A183" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>5</v>
@@ -3908,7 +4649,7 @@
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>5</v>
@@ -3917,7 +4658,7 @@
     </row>
     <row r="185" spans="1:5">
       <c r="A185" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>5</v>
@@ -3926,7 +4667,7 @@
     </row>
     <row r="186" spans="1:5">
       <c r="A186" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>5</v>
@@ -3935,7 +4676,7 @@
     </row>
     <row r="187" spans="1:5">
       <c r="A187" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>5</v>
@@ -3944,7 +4685,7 @@
     </row>
     <row r="188" spans="1:5">
       <c r="A188" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>5</v>
@@ -3953,7 +4694,7 @@
     </row>
     <row r="189" spans="1:5">
       <c r="A189" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>5</v>
@@ -3962,7 +4703,7 @@
     </row>
     <row r="190" spans="1:5">
       <c r="A190" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>5</v>
@@ -3972,7 +4713,7 @@
     </row>
     <row r="191" spans="1:5">
       <c r="A191" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>5</v>
@@ -3982,7 +4723,7 @@
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>5</v>
@@ -3991,7 +4732,7 @@
     </row>
     <row r="193" spans="1:5">
       <c r="A193" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>12</v>
@@ -4000,7 +4741,7 @@
     </row>
     <row r="194" spans="1:5">
       <c r="A194" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>12</v>
@@ -4009,7 +4750,7 @@
     </row>
     <row r="195" spans="1:5">
       <c r="A195" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>12</v>
@@ -4018,7 +4759,7 @@
     </row>
     <row r="196" spans="1:5">
       <c r="A196" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>12</v>
@@ -4027,7 +4768,7 @@
     </row>
     <row r="197" spans="1:5">
       <c r="A197" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>12</v>
@@ -4036,7 +4777,7 @@
     </row>
     <row r="198" spans="1:5">
       <c r="A198" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>12</v>
@@ -4045,7 +4786,7 @@
     </row>
     <row r="199" spans="1:5">
       <c r="A199" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>12</v>
@@ -4054,7 +4795,7 @@
     </row>
     <row r="200" spans="1:5">
       <c r="A200" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>12</v>
@@ -4063,7 +4804,7 @@
     </row>
     <row r="201" spans="1:5">
       <c r="A201" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>12</v>
@@ -4072,7 +4813,7 @@
     </row>
     <row r="202" spans="1:5">
       <c r="A202" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>12</v>
@@ -4082,7 +4823,7 @@
     </row>
     <row r="203" spans="1:5">
       <c r="A203" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>12</v>
@@ -4092,7 +4833,7 @@
     </row>
     <row r="204" spans="1:5">
       <c r="A204" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>12</v>
@@ -4102,7 +4843,7 @@
     </row>
     <row r="205" spans="1:5">
       <c r="A205" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>5</v>
@@ -4111,7 +4852,7 @@
     </row>
     <row r="206" spans="1:5">
       <c r="A206" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>12</v>
@@ -4120,7 +4861,7 @@
     </row>
     <row r="207" spans="1:5">
       <c r="A207" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>5</v>
@@ -4129,7 +4870,7 @@
     </row>
     <row r="208" spans="1:5">
       <c r="A208" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>12</v>
@@ -4138,7 +4879,7 @@
     </row>
     <row r="209" spans="1:5">
       <c r="A209" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>12</v>
@@ -4147,7 +4888,7 @@
     </row>
     <row r="210" spans="1:5">
       <c r="A210" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>12</v>
@@ -4156,7 +4897,7 @@
     </row>
     <row r="211" spans="1:5">
       <c r="A211" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>5</v>
@@ -4165,7 +4906,7 @@
     </row>
     <row r="212" spans="1:5">
       <c r="A212" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>12</v>
@@ -4174,7 +4915,7 @@
     </row>
     <row r="213" spans="1:5">
       <c r="A213" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>5</v>
@@ -4183,7 +4924,7 @@
     </row>
     <row r="214" spans="1:5">
       <c r="A214" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>5</v>
@@ -4192,7 +4933,7 @@
     </row>
     <row r="215" spans="1:5">
       <c r="A215" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>5</v>
@@ -4201,7 +4942,7 @@
     </row>
     <row r="216" spans="1:5">
       <c r="A216" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>5</v>
@@ -4210,7 +4951,7 @@
     </row>
     <row r="217" spans="1:5">
       <c r="A217" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>5</v>
@@ -4220,7 +4961,7 @@
     </row>
     <row r="218" spans="1:5">
       <c r="A218" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>5</v>
@@ -4230,7 +4971,7 @@
     </row>
     <row r="219" spans="1:5">
       <c r="A219" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>5</v>
@@ -4240,7 +4981,7 @@
     </row>
     <row r="220" spans="1:5">
       <c r="A220" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>5</v>
@@ -4249,7 +4990,7 @@
     </row>
     <row r="221" spans="1:5">
       <c r="A221" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>5</v>
@@ -4258,7 +4999,7 @@
     </row>
     <row r="222" spans="1:5">
       <c r="A222" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>5</v>
@@ -4267,7 +5008,7 @@
     </row>
     <row r="223" spans="1:5">
       <c r="A223" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>5</v>
@@ -4276,7 +5017,7 @@
     </row>
     <row r="224" spans="1:5">
       <c r="A224" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>5</v>
@@ -4285,7 +5026,7 @@
     </row>
     <row r="225" spans="1:5">
       <c r="A225" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>12</v>
@@ -4294,7 +5035,7 @@
     </row>
     <row r="226" spans="1:5">
       <c r="A226" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>12</v>
@@ -4303,7 +5044,7 @@
     </row>
     <row r="227" spans="1:5">
       <c r="A227" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>5</v>
@@ -4312,7 +5053,7 @@
     </row>
     <row r="228" spans="1:5">
       <c r="A228" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>5</v>
@@ -4321,7 +5062,7 @@
     </row>
     <row r="229" spans="1:5">
       <c r="A229" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>5</v>
@@ -4330,7 +5071,7 @@
     </row>
     <row r="230" spans="1:5">
       <c r="A230" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>5</v>
@@ -4339,7 +5080,7 @@
     </row>
     <row r="231" spans="1:5">
       <c r="A231" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>5</v>
@@ -4348,7 +5089,7 @@
     </row>
     <row r="232" spans="1:5">
       <c r="A232" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>5</v>
@@ -4357,7 +5098,7 @@
     </row>
     <row r="233" spans="1:5">
       <c r="A233" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>5</v>
@@ -4366,7 +5107,7 @@
     </row>
     <row r="234" spans="1:5">
       <c r="A234" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B234" s="1" t="s">
         <v>5</v>
@@ -4375,7 +5116,7 @@
     </row>
     <row r="235" spans="1:5">
       <c r="A235" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B235" s="1" t="s">
         <v>5</v>
@@ -4385,7 +5126,7 @@
     </row>
     <row r="236" spans="1:5">
       <c r="A236" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B236" s="1" t="s">
         <v>5</v>
@@ -4395,7 +5136,7 @@
     </row>
     <row r="237" spans="1:5">
       <c r="A237" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>5</v>
@@ -4404,7 +5145,7 @@
     </row>
     <row r="238" spans="1:5">
       <c r="A238" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>5</v>
@@ -4413,7 +5154,7 @@
     </row>
     <row r="239" spans="1:5">
       <c r="A239" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B239" s="1" t="s">
         <v>5</v>
@@ -4422,7 +5163,7 @@
     </row>
     <row r="240" spans="1:5">
       <c r="A240" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B240" s="1" t="s">
         <v>5</v>
@@ -4431,7 +5172,7 @@
     </row>
     <row r="241" spans="1:5">
       <c r="A241" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B241" s="1" t="s">
         <v>5</v>
@@ -4440,7 +5181,7 @@
     </row>
     <row r="242" spans="1:5">
       <c r="A242" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B242" s="1" t="s">
         <v>5</v>
@@ -4449,7 +5190,7 @@
     </row>
     <row r="243" spans="1:5">
       <c r="A243" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>5</v>
@@ -4458,7 +5199,7 @@
     </row>
     <row r="244" spans="1:5">
       <c r="A244" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B244" s="1" t="s">
         <v>12</v>
@@ -4467,7 +5208,7 @@
     </row>
     <row r="245" spans="1:5">
       <c r="A245" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B245" s="1" t="s">
         <v>12</v>
@@ -4476,7 +5217,7 @@
     </row>
     <row r="246" spans="1:5">
       <c r="A246" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B246" s="1" t="s">
         <v>12</v>
@@ -4485,7 +5226,7 @@
     </row>
     <row r="247" spans="1:5">
       <c r="A247" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>12</v>
@@ -4494,7 +5235,7 @@
     </row>
     <row r="248" spans="1:5">
       <c r="A248" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>12</v>
@@ -4503,7 +5244,7 @@
     </row>
     <row r="249" spans="1:5">
       <c r="A249" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B249" s="1" t="s">
         <v>12</v>
@@ -4512,7 +5253,7 @@
     </row>
     <row r="250" spans="1:5">
       <c r="A250" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B250" s="1" t="s">
         <v>12</v>
@@ -4522,7 +5263,7 @@
     </row>
     <row r="251" spans="1:5">
       <c r="A251" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B251" s="1" t="s">
         <v>12</v>
@@ -4532,7 +5273,7 @@
     </row>
     <row r="252" spans="1:5">
       <c r="A252" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B252" s="1" t="s">
         <v>5</v>
@@ -4541,7 +5282,7 @@
     </row>
     <row r="253" spans="1:5">
       <c r="A253" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B253" s="1" t="s">
         <v>5</v>
@@ -4550,7 +5291,7 @@
     </row>
     <row r="254" spans="1:5">
       <c r="A254" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B254" s="1" t="s">
         <v>5</v>
@@ -4559,7 +5300,7 @@
     </row>
     <row r="255" spans="1:5">
       <c r="A255" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B255" s="1" t="s">
         <v>5</v>
@@ -4568,7 +5309,7 @@
     </row>
     <row r="256" spans="1:5">
       <c r="A256" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B256" s="1" t="s">
         <v>5</v>
@@ -4577,7 +5318,7 @@
     </row>
     <row r="257" spans="1:5">
       <c r="A257" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B257" s="1" t="s">
         <v>5</v>
@@ -4586,7 +5327,7 @@
     </row>
     <row r="258" spans="1:5">
       <c r="A258" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B258" s="1" t="s">
         <v>12</v>
@@ -4595,7 +5336,7 @@
     </row>
     <row r="259" spans="1:5">
       <c r="A259" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B259" s="1" t="s">
         <v>12</v>
@@ -4604,10 +5345,10 @@
     </row>
     <row r="260" spans="1:5">
       <c r="A260" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C260" s="4"/>
       <c r="D260" s="4"/>
@@ -4615,10 +5356,10 @@
     </row>
     <row r="261" spans="1:5">
       <c r="A261" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B261" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="B261" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="C261" s="5"/>
       <c r="D261" s="5"/>
@@ -4626,10 +5367,10 @@
     </row>
     <row r="262" spans="1:5">
       <c r="A262" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C262" s="4"/>
       <c r="D262" s="4"/>
@@ -4637,10 +5378,10 @@
     </row>
     <row r="263" spans="1:5">
       <c r="A263" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C263" s="5"/>
       <c r="D263" s="5"/>
@@ -4648,10 +5389,10 @@
     </row>
     <row r="264" spans="1:5">
       <c r="A264" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C264" s="5"/>
       <c r="D264" s="5"/>
@@ -4659,10 +5400,10 @@
     </row>
     <row r="265" spans="1:5">
       <c r="A265" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C265" s="5"/>
       <c r="D265" s="5"/>
@@ -4670,10 +5411,10 @@
     </row>
     <row r="266" spans="1:5">
       <c r="A266" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C266" s="5"/>
       <c r="D266" s="5"/>
@@ -4681,10 +5422,10 @@
     </row>
     <row r="267" spans="1:5">
       <c r="A267" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C267" s="5"/>
       <c r="D267" s="5"/>
@@ -4692,10 +5433,10 @@
     </row>
     <row r="268" spans="1:5">
       <c r="A268" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C268" s="5"/>
       <c r="D268" s="5"/>
@@ -4703,7 +5444,7 @@
     </row>
     <row r="269" spans="1:5">
       <c r="A269" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B269" s="1" t="s">
         <v>5</v>
@@ -4712,7 +5453,7 @@
     </row>
     <row r="270" spans="1:5">
       <c r="A270" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>5</v>
@@ -4721,7 +5462,7 @@
     </row>
     <row r="271" spans="1:5">
       <c r="A271" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>5</v>
@@ -4731,7 +5472,7 @@
     </row>
     <row r="272" spans="1:5">
       <c r="A272" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>5</v>
@@ -4741,7 +5482,7 @@
     </row>
     <row r="273" spans="1:5">
       <c r="A273" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>5</v>
@@ -4751,7 +5492,7 @@
     </row>
     <row r="274" spans="1:5">
       <c r="A274" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B274" s="1" t="s">
         <v>5</v>
@@ -4760,7 +5501,7 @@
     </row>
     <row r="275" spans="1:5">
       <c r="A275" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B275" s="1" t="s">
         <v>5</v>
@@ -4769,7 +5510,7 @@
     </row>
     <row r="276" spans="1:5">
       <c r="A276" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B276" s="1" t="s">
         <v>5</v>
@@ -4778,7 +5519,7 @@
     </row>
     <row r="277" spans="1:5">
       <c r="A277" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B277" s="1" t="s">
         <v>5</v>
@@ -4787,7 +5528,7 @@
     </row>
     <row r="278" spans="1:5">
       <c r="A278" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B278" s="1" t="s">
         <v>5</v>
@@ -4796,7 +5537,7 @@
     </row>
     <row r="279" spans="1:5">
       <c r="A279" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B279" s="1" t="s">
         <v>5</v>
@@ -4805,7 +5546,7 @@
     </row>
     <row r="280" spans="1:5">
       <c r="A280" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B280" s="1" t="s">
         <v>5</v>
@@ -4814,7 +5555,7 @@
     </row>
     <row r="281" spans="1:5">
       <c r="A281" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B281" s="1" t="s">
         <v>5</v>
@@ -4823,7 +5564,7 @@
     </row>
     <row r="282" spans="1:5">
       <c r="A282" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B282" s="1" t="s">
         <v>5</v>
@@ -4833,7 +5574,7 @@
     </row>
     <row r="283" spans="1:5">
       <c r="A283" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B283" s="1" t="s">
         <v>12</v>
@@ -4842,7 +5583,7 @@
     </row>
     <row r="284" spans="1:5">
       <c r="A284" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B284" s="1" t="s">
         <v>12</v>
@@ -4851,7 +5592,7 @@
     </row>
     <row r="285" spans="1:5">
       <c r="A285" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B285" s="1" t="s">
         <v>12</v>
@@ -4860,7 +5601,7 @@
     </row>
     <row r="286" spans="1:5">
       <c r="A286" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B286" s="1" t="s">
         <v>12</v>
@@ -4869,7 +5610,7 @@
     </row>
     <row r="287" spans="1:5">
       <c r="A287" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B287" s="1" t="s">
         <v>12</v>
@@ -4878,7 +5619,7 @@
     </row>
     <row r="288" spans="1:5">
       <c r="A288" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B288" s="1" t="s">
         <v>12</v>
@@ -4887,7 +5628,7 @@
     </row>
     <row r="289" spans="1:5">
       <c r="A289" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B289" s="1" t="s">
         <v>12</v>
@@ -4896,7 +5637,7 @@
     </row>
     <row r="290" spans="1:5">
       <c r="A290" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B290" s="1" t="s">
         <v>12</v>
@@ -4906,7 +5647,7 @@
     </row>
     <row r="291" spans="1:5">
       <c r="A291" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B291" s="1" t="s">
         <v>12</v>
@@ -4916,7 +5657,7 @@
     </row>
     <row r="292" spans="1:5">
       <c r="A292" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B292" s="1" t="s">
         <v>5</v>
@@ -4925,7 +5666,7 @@
     </row>
     <row r="293" spans="1:5">
       <c r="A293" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B293" s="1" t="s">
         <v>12</v>
@@ -4934,7 +5675,7 @@
     </row>
     <row r="294" spans="1:5">
       <c r="A294" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B294" s="1" t="s">
         <v>5</v>
@@ -4943,7 +5684,7 @@
     </row>
     <row r="295" spans="1:5">
       <c r="A295" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B295" s="1" t="s">
         <v>5</v>
@@ -4952,7 +5693,7 @@
     </row>
     <row r="296" spans="1:5">
       <c r="A296" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B296" s="1" t="s">
         <v>5</v>
@@ -4961,7 +5702,7 @@
     </row>
     <row r="297" spans="1:5">
       <c r="A297" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B297" s="1" t="s">
         <v>5</v>
@@ -4970,7 +5711,7 @@
     </row>
     <row r="298" spans="1:5">
       <c r="A298" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B298" s="1" t="s">
         <v>5</v>

</xml_diff>